<commit_message>
Reduced loops in Asset selling driver
</commit_message>
<xml_diff>
--- a/AssetSelling/asset_selling_policy_parameters.xlsx
+++ b/AssetSelling/asset_selling_policy_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnascime/Dropbox/PythonProjects/ORF411/github_private/seqdecisionlib_Asset/Asset selling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jade0001\Documents\01 - Vorlesungen\Stochastische Optimierungsprobleme\Powell SDA repo\stochastic-optimization-master\AssetSelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15C2239-7512-A040-BCCB-1AB3553C23EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871A52FD-CC4F-4763-84E9-75FEF6215648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="4440" windowWidth="17740" windowHeight="8960" activeTab="3" xr2:uid="{1DA193D8-6EE7-6A44-BDCF-D14F5A013405}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{1DA193D8-6EE7-6A44-BDCF-D14F5A013405}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>sell_low</t>
   </si>
@@ -193,12 +193,18 @@
   <si>
     <t>DiscountFactor</t>
   </si>
+  <si>
+    <t>track_min</t>
+  </si>
+  <si>
+    <t>track_max</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -564,12 +570,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="73.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="73.296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -577,7 +583,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -585,7 +591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -593,7 +599,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -601,7 +607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="68">
+    <row r="5" spans="1:2" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -609,7 +615,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="51">
+    <row r="6" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -617,17 +623,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="51">
+    <row r="7" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="34">
+    <row r="8" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="34">
+    <row r="9" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -646,12 +652,12 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -661,7 +667,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -672,7 +678,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -685,38 +691,36 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -729,18 +733,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9865D1F9-4F25-7149-9B83-5EBB8C504130}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -754,10 +758,16 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -771,7 +781,13 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -783,16 +799,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B272AC-B9F0-6245-988D-8924FC3BFAF0}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="5" width="13.1640625" customWidth="1"/>
+    <col min="2" max="5" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -824,7 +840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -866,12 +882,12 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>24</v>
       </c>
@@ -882,7 +898,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -896,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -910,7 +926,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
AssetSelling tracking policy as in book
</commit_message>
<xml_diff>
--- a/AssetSelling/asset_selling_policy_parameters.xlsx
+++ b/AssetSelling/asset_selling_policy_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jade0001\Documents\01 - Vorlesungen\Stochastische Optimierungsprobleme\Powell SDA repo\stochastic-optimization-master\AssetSelling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jade0001\Documents\01 - Vorlesungen\Stochastische Optimierungsprobleme\stochastic-optimization\AssetSelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871A52FD-CC4F-4763-84E9-75FEF6215648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961E56C3-53D9-4FF4-84E5-035793D4AE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{1DA193D8-6EE7-6A44-BDCF-D14F5A013405}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{1DA193D8-6EE7-6A44-BDCF-D14F5A013405}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -652,7 +652,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -686,7 +686,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -696,7 +696,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -735,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9865D1F9-4F25-7149-9B83-5EBB8C504130}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B272AC-B9F0-6245-988D-8924FC3BFAF0}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -842,7 +842,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -866,7 +866,7 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="J2">
         <v>40</v>

</xml_diff>

<commit_message>
minor updates to AssetSelling
</commit_message>
<xml_diff>
--- a/AssetSelling/asset_selling_policy_parameters.xlsx
+++ b/AssetSelling/asset_selling_policy_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jade0001\Documents\01 - Vorlesungen\Stochastische Optimierungsprobleme\stochastic-optimization\AssetSelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90183A71-4ABC-4D72-A611-DAF0B1334220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8B52AE-12DC-4C34-9590-159CD20B310A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{1DA193D8-6EE7-6A44-BDCF-D14F5A013405}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1DA193D8-6EE7-6A44-BDCF-D14F5A013405}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,9 +64,6 @@
     <t>Iterations</t>
   </si>
   <si>
-    <t>'full_grid' policy is a grid search over theta values using the high_low policy</t>
-  </si>
-  <si>
     <t>1)</t>
   </si>
   <si>
@@ -80,18 +76,12 @@
     <t>4)</t>
   </si>
   <si>
-    <t>Use 'Sheet2' to set up the parameters for policy 'full_grid'</t>
-  </si>
-  <si>
     <t>5)</t>
   </si>
   <si>
     <t>6)</t>
   </si>
   <si>
-    <t>After setting up the parameters and saving this spreadsheet, just run  'AssetSellingDriverScript'</t>
-  </si>
-  <si>
     <t>TimeHorizon</t>
   </si>
   <si>
@@ -123,9 +113,6 @@
   </si>
   <si>
     <t>The exogenous process  for the asset price P_t is a random walk, where the P_{t+1} = P_t  + normal(mean_t+1, Variance). The mean_{t+1} is also a random variable, that depends on the bias_{t+1}.</t>
-  </si>
-  <si>
-    <t>Use 'Sheet3' to select the policy, the time horizon, the  parameters for the exogenous process (InitialPrice, InitialBias, UpStep, DownStep,Variance) and to determine the number of iterations and how often we should output the cumulative average of the contributions (for the 'full_grid' only)</t>
   </si>
   <si>
     <r>
@@ -180,9 +167,6 @@
     </r>
   </si>
   <si>
-    <t>Possible available policies are: sell_low, track, high_low and full_grid</t>
-  </si>
-  <si>
     <t>Use 'Sheet1' to set up the parameters for policies 'sell_low','track' and 'high_low'</t>
   </si>
   <si>
@@ -199,6 +183,21 @@
   </si>
   <si>
     <t>single</t>
+  </si>
+  <si>
+    <t>Use 'Sheet2' to set up the parameters for the grid search</t>
+  </si>
+  <si>
+    <t>Possible available policies are: sell_low, track and high_low</t>
+  </si>
+  <si>
+    <t>For all policies there is the option to evaluate them once (for a single value of theta) or do a grid search over multiple values of theta</t>
+  </si>
+  <si>
+    <t>After setting up the parameters and saving this spreadsheet, run  all cells in the Jupyter Notebook 'AssetSellingDriverScript'</t>
+  </si>
+  <si>
+    <t>Use 'Sheet3' to select the policy, the time horizon, the  parameters for the exogenous process (InitialPrice, InitialBias, UpStep, DownStep,Variance) and to determine the number of iterations (sample paths). In the column 'Evaluation' specify either 'single' to evaluate a policy a single time for a given parameter value or specify 'grid_search' to try out multiple values (that are specified in 'Sheet2')</t>
   </si>
 </sst>
 </file>
@@ -567,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD3104C-6FB6-3F44-9F46-136694EB3D8F}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -578,68 +577,68 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -653,7 +652,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -684,10 +683,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -759,13 +758,13 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -800,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B272AC-B9F0-6245-988D-8924FC3BFAF0}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -814,25 +813,25 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
@@ -840,19 +839,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -884,18 +883,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>0.9</v>
@@ -909,7 +908,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>0.2</v>
@@ -923,7 +922,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>0</v>

</xml_diff>

<commit_message>
updated Medical Decision problem
</commit_message>
<xml_diff>
--- a/AssetSelling/asset_selling_policy_parameters.xlsx
+++ b/AssetSelling/asset_selling_policy_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jade0001\Documents\01 - Vorlesungen\Stochastische Optimierungsprobleme\stochastic-optimization\AssetSelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56381376-7249-420F-9CAF-6D2EA38E173F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE3417A-E0F1-481E-819B-4D3290CC6736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1DA193D8-6EE7-6A44-BDCF-D14F5A013405}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{1DA193D8-6EE7-6A44-BDCF-D14F5A013405}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -19,10 +19,21 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -651,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7A4EED-C8D5-874D-B8A3-0AA0A4C7040A}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -683,10 +694,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -696,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -736,7 +747,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -769,13 +780,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1">
         <v>20</v>
@@ -784,10 +795,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -799,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B272AC-B9F0-6245-988D-8924FC3BFAF0}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -845,7 +856,7 @@
         <v>35</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -863,7 +874,7 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <v>10</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>